<commit_message>
fixed bulk template missing
</commit_message>
<xml_diff>
--- a/public/downloads/excel/cases_payment_import_template.xlsx
+++ b/public/downloads/excel/cases_payment_import_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Guide\Lab_Bulk_Upload\Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Guide\Lab_Bulk_Upload\Cases_Payment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3812,9 +3812,9 @@
   </sheetPr>
   <dimension ref="A1:X2001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3832,9 +3832,9 @@
     <col min="12" max="13" width="17.85546875" style="6" customWidth="1"/>
     <col min="14" max="14" width="19.5703125" style="6" customWidth="1"/>
     <col min="15" max="15" width="18.42578125" style="6" customWidth="1"/>
-    <col min="16" max="17" width="15" style="6" customWidth="1"/>
-    <col min="18" max="23" width="0" style="3" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="0" style="3" hidden="1"/>
+    <col min="16" max="16" width="15" style="6" customWidth="1"/>
+    <col min="17" max="17" width="31.5703125" style="6" customWidth="1"/>
+    <col min="18" max="24" width="0" style="3" hidden="1" customWidth="1"/>
     <col min="25" max="16384" width="9.140625" style="3" hidden="1"/>
   </cols>
   <sheetData>
@@ -14874,7 +14874,7 @@
     <row r="2000" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="2001" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="7FjrVK8uoTLtQKrQrRAoSQeYcSzwMyr5sYIkhcl9vMyk6GsJq+ptB4CbqC98e1KY1hfp2tzC9YImVOxcnF2RoQ==" saltValue="gUbE7N5rEM9GdRVlTzoq0A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="jfWlIuw/2LJGTWpSNpWop/4+F1ep4hpbu8iuqdpGWw18ArqgjVqTD18jYFFEQhw/VJI9OZSotqy9c5r28tEbYA==" saltValue="xDxx5DW+tTMgpIJ9isB6LQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F500">
       <formula1>"Year,Month,Day"</formula1>
@@ -14895,7 +14895,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N1048576">
       <formula1>"PCR,Antigen,Clinical Diagnosis,Others"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:Q1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P1048576 Q501:Q1048576">
       <formula1>"Paid, Free"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576">
@@ -14933,9 +14933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15252,7 +15250,6 @@
       <c r="G15" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="m+Fyi06VgATBwn43EfmrKNJkh2HABbougplfcgapgrFwW4vKUy8Tw9F6EnT1XWwd42o4yZsxzYLg/VbJrPvjYg==" saltValue="3g1VnFSbJefPZLJ7+dGwEQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -15261,7 +15258,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BY21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AU6" sqref="AU6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18664,8 +18663,6 @@
       <c r="BY21" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="CaP7daMFvRoXMORFeaxIrFbftTbkP4D1+y2J8DqftCPPps5elyYuZZx8zJmLSiNv9MnPo/l8MS4Xvv6IFy2zNQ==" saltValue="7qdPmaiWAYr2yoiziuxt/w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>